<commit_message>
working on itpo replace
</commit_message>
<xml_diff>
--- a/storage/app/public/download-sample-file/sample-users-list.xlsx
+++ b/storage/app/public/download-sample-file/sample-users-list.xlsx
@@ -5,18 +5,18 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\EMIL\Desktop\bdhms-filament\storage\app\public\download-sample-file\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\EMIL\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F9DB393-2BE0-40BF-B21C-51E965162E68}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85ADE203-5453-4991-B36F-6E2427F095FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{DF672DB0-A4B8-4B5B-B375-992FA5135794}"/>
+    <workbookView xWindow="-105" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{DF672DB0-A4B8-4B5B-B375-992FA5135794}"/>
   </bookViews>
   <sheets>
     <sheet name="retailer-importer-example" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'retailer-importer-example'!$B$1:$E$2360</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'retailer-importer-example'!$B$1:$E$2361</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="69">
   <si>
     <t>Name</t>
   </si>
@@ -65,19 +65,184 @@
     <t>MYMVAI02</t>
   </si>
   <si>
-    <t>Rso 02</t>
-  </si>
-  <si>
     <t>rso02@gmail.com</t>
   </si>
   <si>
-    <t>Rso 03</t>
-  </si>
-  <si>
-    <t>MYMVAI01,MYMVAI02</t>
-  </si>
-  <si>
     <t>rso03@gmail.com</t>
+  </si>
+  <si>
+    <t>MYMVAI01</t>
+  </si>
+  <si>
+    <t>Safiqul Islam</t>
+  </si>
+  <si>
+    <t>Saddam</t>
+  </si>
+  <si>
+    <t>MD. RASEL MIA</t>
+  </si>
+  <si>
+    <t>Robin Mia</t>
+  </si>
+  <si>
+    <t>Md. Thouhul Amin</t>
+  </si>
+  <si>
+    <t>MD. Hasan Mia</t>
+  </si>
+  <si>
+    <t>ABUL BASHER RANA</t>
+  </si>
+  <si>
+    <t>Hridoy Mia</t>
+  </si>
+  <si>
+    <t>Md. Hridoy Mia</t>
+  </si>
+  <si>
+    <t>Badiuzzaman</t>
+  </si>
+  <si>
+    <t>Mijan</t>
+  </si>
+  <si>
+    <t>Md. Mamun Mia</t>
+  </si>
+  <si>
+    <t>rso01@gmail.com</t>
+  </si>
+  <si>
+    <t>rso04@gmail.com</t>
+  </si>
+  <si>
+    <t>rso05@gmail.com</t>
+  </si>
+  <si>
+    <t>rso06@gmail.com</t>
+  </si>
+  <si>
+    <t>rso07@gmail.com</t>
+  </si>
+  <si>
+    <t>rso08@gmail.com</t>
+  </si>
+  <si>
+    <t>rso09@gmail.com</t>
+  </si>
+  <si>
+    <t>rso10@gmail.com</t>
+  </si>
+  <si>
+    <t>rso11@gmail.com</t>
+  </si>
+  <si>
+    <t>rso12@gmail.com</t>
+  </si>
+  <si>
+    <t>rso13@gmail.com</t>
+  </si>
+  <si>
+    <t>rso14@gmail.com</t>
+  </si>
+  <si>
+    <t>rso15@gmail.com</t>
+  </si>
+  <si>
+    <t>rso16@gmail.com</t>
+  </si>
+  <si>
+    <t>rso17@gmail.com</t>
+  </si>
+  <si>
+    <t>rso18@gmail.com</t>
+  </si>
+  <si>
+    <t>rso19@gmail.com</t>
+  </si>
+  <si>
+    <t>rso20@gmail.com</t>
+  </si>
+  <si>
+    <t>rso21@gmail.com</t>
+  </si>
+  <si>
+    <t>rso22@gmail.com</t>
+  </si>
+  <si>
+    <t>rso23@gmail.com</t>
+  </si>
+  <si>
+    <t>rso24@gmail.com</t>
+  </si>
+  <si>
+    <t>rso25@gmail.com</t>
+  </si>
+  <si>
+    <t>Titu Mia</t>
+  </si>
+  <si>
+    <t>Ruhul Amin</t>
+  </si>
+  <si>
+    <t>Mobashir Ahmed</t>
+  </si>
+  <si>
+    <t>supervisor01@gmail.com</t>
+  </si>
+  <si>
+    <t>supervisor02@gmail.com</t>
+  </si>
+  <si>
+    <t>supervisor03@gmail.com</t>
+  </si>
+  <si>
+    <t>supervisor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Md Rajib Miah (Alternate BP)	</t>
+  </si>
+  <si>
+    <t>rso26@gmail.com</t>
+  </si>
+  <si>
+    <t>MD. ALI HOSSAIN</t>
+  </si>
+  <si>
+    <t>Md. Golam Mostufa</t>
+  </si>
+  <si>
+    <t>RIPON RANA</t>
+  </si>
+  <si>
+    <t>MD POROSH MIAH</t>
+  </si>
+  <si>
+    <t>MAHMUD HASAN EMON</t>
+  </si>
+  <si>
+    <t>MD MIJANUR RAHMAN</t>
+  </si>
+  <si>
+    <t>SAHADAT HOSSAIN</t>
+  </si>
+  <si>
+    <t>Hossain Bhuyan</t>
+  </si>
+  <si>
+    <t>RIAZ AHMED</t>
+  </si>
+  <si>
+    <t>FERDOUS MIA</t>
+  </si>
+  <si>
+    <t>MD MOKHTAKIN</t>
+  </si>
+  <si>
+    <t>Md. Shahin mia</t>
+  </si>
+  <si>
+    <t>Opi Ahmed Shuvo</t>
   </si>
 </sst>
 </file>
@@ -625,7 +790,38 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="3">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -955,20 +1151,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6658030-BA40-4FD6-833B-C59E793ABA82}">
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:F30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.85546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="4.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -993,16 +1189,16 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="B2" t="s">
-        <v>9</v>
+        <v>56</v>
       </c>
       <c r="C2">
-        <v>1915000002</v>
+        <v>1711000001</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>10</v>
+        <v>24</v>
       </c>
       <c r="E2" t="s">
         <v>4</v>
@@ -1013,29 +1209,580 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" t="s">
         <v>12</v>
       </c>
-      <c r="B3" t="s">
-        <v>11</v>
-      </c>
       <c r="C3">
-        <v>1915000003</v>
+        <v>1711000002</v>
       </c>
       <c r="D3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" t="s">
         <v>13</v>
       </c>
-      <c r="E3" t="s">
-        <v>4</v>
-      </c>
-      <c r="F3" t="s">
-        <v>6</v>
+      <c r="C4">
+        <v>1711000003</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E4" t="s">
+        <v>4</v>
+      </c>
+      <c r="F4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C5">
+        <v>1711000004</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E5" t="s">
+        <v>4</v>
+      </c>
+      <c r="F5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" t="s">
+        <v>57</v>
+      </c>
+      <c r="C6">
+        <v>1711000005</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E6" t="s">
+        <v>4</v>
+      </c>
+      <c r="F6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" t="s">
+        <v>58</v>
+      </c>
+      <c r="C7">
+        <v>1711000006</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E7" t="s">
+        <v>4</v>
+      </c>
+      <c r="F7" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8">
+        <v>1711000007</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E8" t="s">
+        <v>4</v>
+      </c>
+      <c r="F8" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B9" t="s">
+        <v>15</v>
+      </c>
+      <c r="C9">
+        <v>1711000008</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E9" t="s">
+        <v>4</v>
+      </c>
+      <c r="F9" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>11</v>
+      </c>
+      <c r="B10" t="s">
+        <v>16</v>
+      </c>
+      <c r="C10">
+        <v>1711000009</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E10" t="s">
+        <v>4</v>
+      </c>
+      <c r="F10" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>11</v>
+      </c>
+      <c r="B11" t="s">
+        <v>59</v>
+      </c>
+      <c r="C11">
+        <v>1711000010</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E11" t="s">
+        <v>4</v>
+      </c>
+      <c r="F11" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>17</v>
+      </c>
+      <c r="C12">
+        <v>1711000011</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E12" t="s">
+        <v>4</v>
+      </c>
+      <c r="F12" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>11</v>
+      </c>
+      <c r="B13" t="s">
+        <v>18</v>
+      </c>
+      <c r="C13">
+        <v>1711000012</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E13" t="s">
+        <v>4</v>
+      </c>
+      <c r="F13" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>11</v>
+      </c>
+      <c r="B14" t="s">
+        <v>60</v>
+      </c>
+      <c r="C14">
+        <v>1711000013</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E14" t="s">
+        <v>4</v>
+      </c>
+      <c r="F14" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>11</v>
+      </c>
+      <c r="B15" t="s">
+        <v>61</v>
+      </c>
+      <c r="C15">
+        <v>1711000014</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E15" t="s">
+        <v>4</v>
+      </c>
+      <c r="F15" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>11</v>
+      </c>
+      <c r="B16" t="s">
+        <v>19</v>
+      </c>
+      <c r="C16">
+        <v>1711000015</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E16" t="s">
+        <v>4</v>
+      </c>
+      <c r="F16" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>11</v>
+      </c>
+      <c r="B17" t="s">
+        <v>20</v>
+      </c>
+      <c r="C17">
+        <v>1711000016</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E17" t="s">
+        <v>4</v>
+      </c>
+      <c r="F17" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>11</v>
+      </c>
+      <c r="B18" t="s">
+        <v>62</v>
+      </c>
+      <c r="C18">
+        <v>1711000017</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E18" t="s">
+        <v>4</v>
+      </c>
+      <c r="F18" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>11</v>
+      </c>
+      <c r="B19" t="s">
+        <v>22</v>
+      </c>
+      <c r="C19">
+        <v>1711000018</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E19" t="s">
+        <v>4</v>
+      </c>
+      <c r="F19" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>8</v>
+      </c>
+      <c r="B20" t="s">
+        <v>63</v>
+      </c>
+      <c r="C20">
+        <v>1711000019</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E20" t="s">
+        <v>4</v>
+      </c>
+      <c r="F20" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>8</v>
+      </c>
+      <c r="B21" t="s">
+        <v>23</v>
+      </c>
+      <c r="C21">
+        <v>1711000020</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="E21" t="s">
+        <v>4</v>
+      </c>
+      <c r="F21" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>8</v>
+      </c>
+      <c r="B22" t="s">
+        <v>64</v>
+      </c>
+      <c r="C22">
+        <v>1711000021</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E22" t="s">
+        <v>4</v>
+      </c>
+      <c r="F22" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>8</v>
+      </c>
+      <c r="B23" t="s">
+        <v>65</v>
+      </c>
+      <c r="C23">
+        <v>1711000022</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="E23" t="s">
+        <v>4</v>
+      </c>
+      <c r="F23" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>8</v>
+      </c>
+      <c r="B24" t="s">
+        <v>66</v>
+      </c>
+      <c r="C24">
+        <v>1711000023</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="E24" t="s">
+        <v>4</v>
+      </c>
+      <c r="F24" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>8</v>
+      </c>
+      <c r="B25" t="s">
+        <v>67</v>
+      </c>
+      <c r="C25">
+        <v>1711000024</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="E25" t="s">
+        <v>4</v>
+      </c>
+      <c r="F25" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>8</v>
+      </c>
+      <c r="B26" t="s">
+        <v>68</v>
+      </c>
+      <c r="C26">
+        <v>1711000025</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="E26" t="s">
+        <v>4</v>
+      </c>
+      <c r="F26" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>11</v>
+      </c>
+      <c r="B27" t="s">
+        <v>54</v>
+      </c>
+      <c r="C27">
+        <v>1711000026</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="E27" t="s">
+        <v>4</v>
+      </c>
+      <c r="F27" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>11</v>
+      </c>
+      <c r="B28" t="s">
+        <v>47</v>
+      </c>
+      <c r="C28">
+        <v>1923909896</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="E28" t="s">
+        <v>4</v>
+      </c>
+      <c r="F28" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>11</v>
+      </c>
+      <c r="B29" t="s">
+        <v>48</v>
+      </c>
+      <c r="C29">
+        <v>1911266077</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="E29" t="s">
+        <v>4</v>
+      </c>
+      <c r="F29" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>8</v>
+      </c>
+      <c r="B30" t="s">
+        <v>49</v>
+      </c>
+      <c r="C30">
+        <v>1923909897</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="E30" t="s">
+        <v>4</v>
+      </c>
+      <c r="F30" t="s">
+        <v>53</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
+  <conditionalFormatting sqref="C1:C28 C30:C1048576">
+    <cfRule type="duplicateValues" dxfId="2" priority="3"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G29">
+    <cfRule type="duplicateValues" dxfId="1" priority="2"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C29">
+    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
+  </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1" xr:uid="{1E02F4C6-D4C4-45F5-A010-5ACF69501F2E}"/>
-    <hyperlink ref="D3" r:id="rId2" xr:uid="{E06016CD-3DEA-4CA3-8024-A9598EFA5D47}"/>
+    <hyperlink ref="D28" r:id="rId1" xr:uid="{E26A99D9-BB83-4396-A566-127B09CEDFCE}"/>
+    <hyperlink ref="D29" r:id="rId2" xr:uid="{D4146FB0-E99C-4360-879B-A763F638ECF9}"/>
+    <hyperlink ref="D30" r:id="rId3" xr:uid="{961FFA85-4351-45D2-BE41-0AF5544A447D}"/>
+    <hyperlink ref="D27" r:id="rId4" xr:uid="{335159E9-5528-49E7-8AE8-147624757BBA}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>